<commit_message>
PQ Challenge 102 file has been modified.
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ  Challenge 102 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ  Challenge 102 Problem.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31EEBE3-9109-459B-B020-6A4B44FF6F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE8D6B1-663B-4CEE-9092-67A3A6619833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="34580" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="134">
   <si>
     <t>Dept</t>
   </si>
@@ -464,6 +465,9 @@
   </si>
   <si>
     <t>Robert,X</t>
+  </si>
+  <si>
+    <t>AX</t>
   </si>
 </sst>
 </file>
@@ -495,7 +499,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +521,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -644,6 +660,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,7 +1269,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="11">
+  <wetp:taskpane dockstate="right" visibility="0" width="1736" row="12">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1286,8 +1304,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,7 +1380,7 @@
         <v>Name</v>
       </c>
       <c r="Q2" t="str" cm="1">
-        <f t="array" ref="Q2:V64">_xlfn.LAMBDA(_xlpm.Vector, _xlfn.LET(_xlpm.AllCombo, _xlfn.DROP(_xlfn.REDUCE("", _xlpm.Vector, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.LET(_xlpm.CurrExpanded, _xlfn.EXPAND(_xlpm.Curr, ROWS(_xlpm.Acc), , _xlpm.Curr), _xlpm.HorizontalStack, _xlfn.HSTACK(_xlpm.Acc, _xlpm.CurrExpanded), _xlpm.StackVeritcally, _xlfn.VSTACK(_xlpm.Acc, _xlpm.HorizontalStack), _xlpm.Result, _xlfn.IFNA(_xlpm.StackVeritcally, ""), _xlpm.Result))), 1, 1), _xlpm.Seq, _xlfn.SEQUENCE(ROWS(_xlpm.AllCombo)), _xlpm.LeftShifted, _xlfn.DROP(_xlfn.REDUCE("", _xlpm.Seq, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.LET(_xlpm.RowData, _xlfn.CHOOSEROWS(_xlpm.AllCombo, _xlpm.Curr), _xlpm.BlankRemoved, _xlfn._xlws.FILTER(_xlpm.RowData, _xlpm.RowData &lt;&gt; ""), _xlpm.MakeSameSize, _xlfn.HSTACK(_xlfn.EXPAND(_xlpm.BlankRemoved, 1, COLUMNS(_xlpm.AllCombo), ""), COLUMNS(_xlpm.BlankRemoved)), _xlpm.Result, _xlfn.VSTACK(_xlpm.Acc, _xlpm.MakeSameSize), _xlpm.Result))), 1), _xlpm.IndexInMainVector, _xlfn.XMATCH(_xlfn.TAKE(_xlpm.LeftShifted, , 1), _xlpm.Vector, 0), _xlpm.SortByItemCount, _xlfn.SORTBY(_xlfn.DROP(_xlpm.LeftShifted, , -1), _xlpm.IndexInMainVector, 1, _xlfn.TAKE(_xlpm.LeftShifted, , -1), 1), _xlpm.SortByItemCount))({"A","B","C","D","E","F"})</f>
+        <f t="array" ref="Q2:V64">_xlfn.LAMBDA(_xlpm.Vector, _xlfn.LET(_xlpm.AllCombo, _xlfn.DROP(_xlfn.REDUCE("", _xlpm.Vector, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.LET(_xlpm.CurrExpanded, _xlfn.EXPAND(_xlpm.Curr, ROWS(_xlpm.Acc), , _xlpm.Curr), _xlpm.HorizontalStack, _xlfn.HSTACK(_xlpm.Acc, _xlpm.CurrExpanded), _xlpm.StackVeritcally, _xlfn.VSTACK(_xlpm.Acc, _xlpm.HorizontalStack), _xlpm.Result, _xlfn.IFNA(_xlpm.StackVeritcally, ""), _xlpm.Result))), 1, 1), _xlpm.Seq, _xlfn.SEQUENCE(ROWS(_xlpm.AllCombo)), _xlpm.LeftShifted, _xlfn.DROP(_xlfn.REDUCE("", _xlpm.Seq, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.LET(_xlpm.RowData, _xlfn.CHOOSEROWS(_xlpm.AllCombo, _xlpm.Curr), _xlpm.BlankRemoved, _xlfn._xlws.FILTER(_xlpm.RowData, _xlpm.RowData &lt;&gt; ""), _xlpm.MakeSameSize, _xlfn.HSTACK(_xlfn.EXPAND(_xlpm.BlankRemoved, 1, COLUMNS(_xlpm.AllCombo), ""), COLUMNS(_xlpm.BlankRemoved)), _xlpm.Result, _xlfn.VSTACK(_xlpm.Acc, _xlpm.MakeSameSize), _xlpm.Result))), 1), _xlpm.IndexInMainVector, _xlfn.XMATCH(_xlfn.TAKE(_xlpm.LeftShifted, , 1), _xlpm.Vector, 0), _xlpm.SortByItemCount, _xlfn.SORTBY(_xlfn.DROP(_xlpm.LeftShifted, , -1), _xlpm.IndexInMainVector, 1, _xlfn.TAKE(_xlpm.LeftShifted, , -1), 1), _xlpm.AllCombo))({"A","B","C","D","E","F"})</f>
         <v>A</v>
       </c>
       <c r="R2" t="str">
@@ -1414,7 +1432,7 @@
         <v>Mary</v>
       </c>
       <c r="Q3" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R3" t="str">
         <v>B</v>
@@ -1467,7 +1485,7 @@
         <v>A</v>
       </c>
       <c r="R4" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="S4" t="str">
         <v/>
@@ -1514,13 +1532,13 @@
         <v>Mary, Robert, Patricia</v>
       </c>
       <c r="Q5" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R5" t="str">
-        <v>D</v>
+        <v/>
       </c>
       <c r="S5" t="str">
-        <v/>
+        <v>C</v>
       </c>
       <c r="T5" t="str">
         <v/>
@@ -1567,10 +1585,10 @@
         <v>A</v>
       </c>
       <c r="R6" t="str">
-        <v>E</v>
+        <v/>
       </c>
       <c r="S6" t="str">
-        <v/>
+        <v>C</v>
       </c>
       <c r="T6" t="str">
         <v/>
@@ -1614,13 +1632,13 @@
         <v>Mary, Robert, Patricia, John, Jennifer</v>
       </c>
       <c r="Q7" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R7" t="str">
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="S7" t="str">
-        <v/>
+        <v>C</v>
       </c>
       <c r="T7" t="str">
         <v/>
@@ -1702,16 +1720,16 @@
         <v>Mary, Robert, John</v>
       </c>
       <c r="Q9" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R9" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S9" t="str">
+        <v/>
+      </c>
+      <c r="T9" t="str">
         <v>D</v>
-      </c>
-      <c r="T9" t="str">
-        <v/>
       </c>
       <c r="U9" t="str">
         <v/>
@@ -1749,13 +1767,13 @@
         <v>A</v>
       </c>
       <c r="R10" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="S10" t="str">
+        <v/>
+      </c>
+      <c r="T10" t="str">
         <v>D</v>
-      </c>
-      <c r="T10" t="str">
-        <v/>
       </c>
       <c r="U10" t="str">
         <v/>
@@ -1790,16 +1808,16 @@
         <v>Mary, Robert, Jennifer</v>
       </c>
       <c r="Q11" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R11" t="str">
         <v>B</v>
       </c>
       <c r="S11" t="str">
-        <v>E</v>
+        <v/>
       </c>
       <c r="T11" t="str">
-        <v/>
+        <v>D</v>
       </c>
       <c r="U11" t="str">
         <v/>
@@ -1837,13 +1855,13 @@
         <v>A</v>
       </c>
       <c r="R12" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="S12" t="str">
-        <v>E</v>
+        <v/>
       </c>
       <c r="T12" t="str">
-        <v/>
+        <v>D</v>
       </c>
       <c r="U12" t="str">
         <v/>
@@ -1878,16 +1896,16 @@
         <v>Mary, Patricia, John</v>
       </c>
       <c r="Q13" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R13" t="str">
+        <v/>
+      </c>
+      <c r="S13" t="str">
+        <v>C</v>
+      </c>
+      <c r="T13" t="str">
         <v>D</v>
-      </c>
-      <c r="S13" t="str">
-        <v>E</v>
-      </c>
-      <c r="T13" t="str">
-        <v/>
       </c>
       <c r="U13" t="str">
         <v/>
@@ -1925,13 +1943,13 @@
         <v>A</v>
       </c>
       <c r="R14" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S14" t="str">
-        <v>F</v>
+        <v>C</v>
       </c>
       <c r="T14" t="str">
-        <v/>
+        <v>D</v>
       </c>
       <c r="U14" t="str">
         <v/>
@@ -1966,16 +1984,16 @@
         <v>Mary, Patricia, Jennifer</v>
       </c>
       <c r="Q15" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R15" t="str">
+        <v>B</v>
+      </c>
+      <c r="S15" t="str">
         <v>C</v>
       </c>
-      <c r="S15" t="str">
-        <v>F</v>
-      </c>
       <c r="T15" t="str">
-        <v/>
+        <v>D</v>
       </c>
       <c r="U15" t="str">
         <v/>
@@ -2013,13 +2031,13 @@
         <v>A</v>
       </c>
       <c r="R16" t="str">
+        <v>B</v>
+      </c>
+      <c r="S16" t="str">
+        <v>C</v>
+      </c>
+      <c r="T16" t="str">
         <v>D</v>
-      </c>
-      <c r="S16" t="str">
-        <v>F</v>
-      </c>
-      <c r="T16" t="str">
-        <v/>
       </c>
       <c r="U16" t="str">
         <v/>
@@ -2054,19 +2072,19 @@
         <v>Mary, John, Jennifer</v>
       </c>
       <c r="Q17" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R17" t="str">
+        <v/>
+      </c>
+      <c r="S17" t="str">
+        <v/>
+      </c>
+      <c r="T17" t="str">
+        <v/>
+      </c>
+      <c r="U17" t="str">
         <v>E</v>
-      </c>
-      <c r="S17" t="str">
-        <v>F</v>
-      </c>
-      <c r="T17" t="str">
-        <v/>
-      </c>
-      <c r="U17" t="str">
-        <v/>
       </c>
       <c r="V17" t="str">
         <v/>
@@ -2101,16 +2119,16 @@
         <v>A</v>
       </c>
       <c r="R18" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S18" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="T18" t="str">
-        <v>D</v>
+        <v/>
       </c>
       <c r="U18" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V18" t="str">
         <v/>
@@ -2142,19 +2160,19 @@
         <v>James</v>
       </c>
       <c r="Q19" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R19" t="str">
         <v>B</v>
       </c>
       <c r="S19" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="T19" t="str">
+        <v/>
+      </c>
+      <c r="U19" t="str">
         <v>E</v>
-      </c>
-      <c r="U19" t="str">
-        <v/>
       </c>
       <c r="V19" t="str">
         <v/>
@@ -2192,13 +2210,13 @@
         <v>B</v>
       </c>
       <c r="S20" t="str">
-        <v>D</v>
+        <v/>
       </c>
       <c r="T20" t="str">
+        <v/>
+      </c>
+      <c r="U20" t="str">
         <v>E</v>
-      </c>
-      <c r="U20" t="str">
-        <v/>
       </c>
       <c r="V20" t="str">
         <v/>
@@ -2230,19 +2248,19 @@
         <v>James, Mary, Robert</v>
       </c>
       <c r="Q21" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R21" t="str">
+        <v/>
+      </c>
+      <c r="S21" t="str">
         <v>C</v>
       </c>
-      <c r="S21" t="str">
-        <v>D</v>
-      </c>
       <c r="T21" t="str">
+        <v/>
+      </c>
+      <c r="U21" t="str">
         <v>E</v>
-      </c>
-      <c r="U21" t="str">
-        <v/>
       </c>
       <c r="V21" t="str">
         <v/>
@@ -2277,16 +2295,16 @@
         <v>A</v>
       </c>
       <c r="R22" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S22" t="str">
         <v>C</v>
       </c>
       <c r="T22" t="str">
-        <v>F</v>
+        <v/>
       </c>
       <c r="U22" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V22" t="str">
         <v/>
@@ -2318,19 +2336,19 @@
         <v>James, Mary, Robert, Patricia, John</v>
       </c>
       <c r="Q23" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R23" t="str">
         <v>B</v>
       </c>
       <c r="S23" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="T23" t="str">
-        <v>F</v>
+        <v/>
       </c>
       <c r="U23" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V23" t="str">
         <v/>
@@ -2365,16 +2383,16 @@
         <v>A</v>
       </c>
       <c r="R24" t="str">
+        <v>B</v>
+      </c>
+      <c r="S24" t="str">
         <v>C</v>
       </c>
-      <c r="S24" t="str">
-        <v>D</v>
-      </c>
       <c r="T24" t="str">
-        <v>F</v>
+        <v/>
       </c>
       <c r="U24" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V24" t="str">
         <v/>
@@ -2406,19 +2424,19 @@
         <v>James, Mary, Robert, Patricia, Jennifer</v>
       </c>
       <c r="Q25" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R25" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S25" t="str">
+        <v/>
+      </c>
+      <c r="T25" t="str">
+        <v>D</v>
+      </c>
+      <c r="U25" t="str">
         <v>E</v>
-      </c>
-      <c r="T25" t="str">
-        <v>F</v>
-      </c>
-      <c r="U25" t="str">
-        <v/>
       </c>
       <c r="V25" t="str">
         <v/>
@@ -2453,16 +2471,16 @@
         <v>A</v>
       </c>
       <c r="R26" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="S26" t="str">
+        <v/>
+      </c>
+      <c r="T26" t="str">
+        <v>D</v>
+      </c>
+      <c r="U26" t="str">
         <v>E</v>
-      </c>
-      <c r="T26" t="str">
-        <v>F</v>
-      </c>
-      <c r="U26" t="str">
-        <v/>
       </c>
       <c r="V26" t="str">
         <v/>
@@ -2494,19 +2512,19 @@
         <v>James, Mary, Robert, John, Jennifer</v>
       </c>
       <c r="Q27" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R27" t="str">
+        <v>B</v>
+      </c>
+      <c r="S27" t="str">
+        <v/>
+      </c>
+      <c r="T27" t="str">
         <v>D</v>
       </c>
-      <c r="S27" t="str">
+      <c r="U27" t="str">
         <v>E</v>
-      </c>
-      <c r="T27" t="str">
-        <v>F</v>
-      </c>
-      <c r="U27" t="str">
-        <v/>
       </c>
       <c r="V27" t="str">
         <v/>
@@ -2544,7 +2562,7 @@
         <v>B</v>
       </c>
       <c r="S28" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="T28" t="str">
         <v>D</v>
@@ -2582,10 +2600,10 @@
         <v>James, Mary, Patricia</v>
       </c>
       <c r="Q29" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R29" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S29" t="str">
         <v>C</v>
@@ -2594,7 +2612,7 @@
         <v>D</v>
       </c>
       <c r="U29" t="str">
-        <v>F</v>
+        <v>E</v>
       </c>
       <c r="V29" t="str">
         <v/>
@@ -2629,16 +2647,16 @@
         <v>A</v>
       </c>
       <c r="R30" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S30" t="str">
         <v>C</v>
       </c>
       <c r="T30" t="str">
+        <v>D</v>
+      </c>
+      <c r="U30" t="str">
         <v>E</v>
-      </c>
-      <c r="U30" t="str">
-        <v>F</v>
       </c>
       <c r="V30" t="str">
         <v/>
@@ -2670,19 +2688,19 @@
         <v>James, Mary, Patricia, John, Jennifer</v>
       </c>
       <c r="Q31" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R31" t="str">
         <v>B</v>
       </c>
       <c r="S31" t="str">
+        <v>C</v>
+      </c>
+      <c r="T31" t="str">
         <v>D</v>
       </c>
-      <c r="T31" t="str">
+      <c r="U31" t="str">
         <v>E</v>
-      </c>
-      <c r="U31" t="str">
-        <v>F</v>
       </c>
       <c r="V31" t="str">
         <v/>
@@ -2717,16 +2735,16 @@
         <v>A</v>
       </c>
       <c r="R32" t="str">
+        <v>B</v>
+      </c>
+      <c r="S32" t="str">
         <v>C</v>
       </c>
-      <c r="S32" t="str">
+      <c r="T32" t="str">
         <v>D</v>
       </c>
-      <c r="T32" t="str">
+      <c r="U32" t="str">
         <v>E</v>
-      </c>
-      <c r="U32" t="str">
-        <v>F</v>
       </c>
       <c r="V32" t="str">
         <v/>
@@ -2758,19 +2776,19 @@
         <v>James, Mary, John</v>
       </c>
       <c r="Q33" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="R33" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="S33" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="T33" t="str">
-        <v>D</v>
+        <v/>
       </c>
       <c r="U33" t="str">
-        <v>E</v>
+        <v/>
       </c>
       <c r="V33" t="str">
         <v>F</v>
@@ -2802,7 +2820,7 @@
         <v>James, Mary, John, Jennifer</v>
       </c>
       <c r="Q34" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="R34" t="str">
         <v/>
@@ -2817,7 +2835,7 @@
         <v/>
       </c>
       <c r="V34" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X34" t="str">
         <v>B</v>
@@ -2846,11 +2864,11 @@
         <v>James, Mary, Jennifer</v>
       </c>
       <c r="Q35" t="str">
+        <v/>
+      </c>
+      <c r="R35" t="str">
         <v>B</v>
       </c>
-      <c r="R35" t="str">
-        <v>C</v>
-      </c>
       <c r="S35" t="str">
         <v/>
       </c>
@@ -2861,7 +2879,7 @@
         <v/>
       </c>
       <c r="V35" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X35" t="str">
         <v>B, C</v>
@@ -2890,11 +2908,11 @@
         <v>James, Robert</v>
       </c>
       <c r="Q36" t="str">
+        <v>A</v>
+      </c>
+      <c r="R36" t="str">
         <v>B</v>
       </c>
-      <c r="R36" t="str">
-        <v>D</v>
-      </c>
       <c r="S36" t="str">
         <v/>
       </c>
@@ -2905,7 +2923,7 @@
         <v/>
       </c>
       <c r="V36" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X36" t="str">
         <v>B, D</v>
@@ -2934,13 +2952,13 @@
         <v>James, Robert, Patricia</v>
       </c>
       <c r="Q37" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="R37" t="str">
-        <v>E</v>
+        <v/>
       </c>
       <c r="S37" t="str">
-        <v/>
+        <v>C</v>
       </c>
       <c r="T37" t="str">
         <v/>
@@ -2949,7 +2967,7 @@
         <v/>
       </c>
       <c r="V37" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X37" t="str">
         <v>B, E</v>
@@ -2978,22 +2996,22 @@
         <v>James, Robert, Patricia, John</v>
       </c>
       <c r="Q38" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="R38" t="str">
+        <v/>
+      </c>
+      <c r="S38" t="str">
+        <v>C</v>
+      </c>
+      <c r="T38" t="str">
+        <v/>
+      </c>
+      <c r="U38" t="str">
+        <v/>
+      </c>
+      <c r="V38" t="str">
         <v>F</v>
-      </c>
-      <c r="S38" t="str">
-        <v/>
-      </c>
-      <c r="T38" t="str">
-        <v/>
-      </c>
-      <c r="U38" t="str">
-        <v/>
-      </c>
-      <c r="V38" t="str">
-        <v/>
       </c>
       <c r="X38" t="str">
         <v>B, F</v>
@@ -3022,14 +3040,14 @@
         <v>James, Robert, Patricia, John, Jennifer</v>
       </c>
       <c r="Q39" t="str">
+        <v/>
+      </c>
+      <c r="R39" t="str">
         <v>B</v>
       </c>
-      <c r="R39" t="str">
+      <c r="S39" t="str">
         <v>C</v>
       </c>
-      <c r="S39" t="str">
-        <v>D</v>
-      </c>
       <c r="T39" t="str">
         <v/>
       </c>
@@ -3037,7 +3055,7 @@
         <v/>
       </c>
       <c r="V39" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X39" t="str">
         <v>B, C, D</v>
@@ -3066,14 +3084,14 @@
         <v>James, Robert, Patricia, Jennifer</v>
       </c>
       <c r="Q40" t="str">
+        <v>A</v>
+      </c>
+      <c r="R40" t="str">
         <v>B</v>
       </c>
-      <c r="R40" t="str">
+      <c r="S40" t="str">
         <v>C</v>
       </c>
-      <c r="S40" t="str">
-        <v>E</v>
-      </c>
       <c r="T40" t="str">
         <v/>
       </c>
@@ -3081,7 +3099,7 @@
         <v/>
       </c>
       <c r="V40" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X40" t="str">
         <v>B, C, E</v>
@@ -3110,22 +3128,22 @@
         <v>James, Robert, John</v>
       </c>
       <c r="Q41" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="R41" t="str">
+        <v/>
+      </c>
+      <c r="S41" t="str">
+        <v/>
+      </c>
+      <c r="T41" t="str">
         <v>D</v>
       </c>
-      <c r="S41" t="str">
-        <v>E</v>
-      </c>
-      <c r="T41" t="str">
-        <v/>
-      </c>
       <c r="U41" t="str">
         <v/>
       </c>
       <c r="V41" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X41" t="str">
         <v>B, C, F</v>
@@ -3154,22 +3172,22 @@
         <v>James, Robert, John, Jennifer</v>
       </c>
       <c r="Q42" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="R42" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="S42" t="str">
+        <v/>
+      </c>
+      <c r="T42" t="str">
+        <v>D</v>
+      </c>
+      <c r="U42" t="str">
+        <v/>
+      </c>
+      <c r="V42" t="str">
         <v>F</v>
-      </c>
-      <c r="T42" t="str">
-        <v/>
-      </c>
-      <c r="U42" t="str">
-        <v/>
-      </c>
-      <c r="V42" t="str">
-        <v/>
       </c>
       <c r="X42" t="str">
         <v>B, D, E</v>
@@ -3198,22 +3216,22 @@
         <v>James, Robert, Jennifer</v>
       </c>
       <c r="Q43" t="str">
+        <v/>
+      </c>
+      <c r="R43" t="str">
         <v>B</v>
       </c>
-      <c r="R43" t="str">
+      <c r="S43" t="str">
+        <v/>
+      </c>
+      <c r="T43" t="str">
         <v>D</v>
       </c>
-      <c r="S43" t="str">
+      <c r="U43" t="str">
+        <v/>
+      </c>
+      <c r="V43" t="str">
         <v>F</v>
-      </c>
-      <c r="T43" t="str">
-        <v/>
-      </c>
-      <c r="U43" t="str">
-        <v/>
-      </c>
-      <c r="V43" t="str">
-        <v/>
       </c>
       <c r="X43" t="str">
         <v>B, D, F</v>
@@ -3242,22 +3260,22 @@
         <v>James, Patricia</v>
       </c>
       <c r="Q44" t="str">
+        <v>A</v>
+      </c>
+      <c r="R44" t="str">
         <v>B</v>
       </c>
-      <c r="R44" t="str">
-        <v>E</v>
-      </c>
       <c r="S44" t="str">
+        <v/>
+      </c>
+      <c r="T44" t="str">
+        <v>D</v>
+      </c>
+      <c r="U44" t="str">
+        <v/>
+      </c>
+      <c r="V44" t="str">
         <v>F</v>
-      </c>
-      <c r="T44" t="str">
-        <v/>
-      </c>
-      <c r="U44" t="str">
-        <v/>
-      </c>
-      <c r="V44" t="str">
-        <v/>
       </c>
       <c r="X44" t="str">
         <v>B, E, F</v>
@@ -3286,22 +3304,22 @@
         <v>James, Patricia, John</v>
       </c>
       <c r="Q45" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="R45" t="str">
+        <v/>
+      </c>
+      <c r="S45" t="str">
         <v>C</v>
       </c>
-      <c r="S45" t="str">
+      <c r="T45" t="str">
         <v>D</v>
       </c>
-      <c r="T45" t="str">
-        <v>E</v>
-      </c>
       <c r="U45" t="str">
         <v/>
       </c>
       <c r="V45" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X45" t="str">
         <v>B, C, D, E</v>
@@ -3330,22 +3348,22 @@
         <v>James, Patricia, John, Jennifer</v>
       </c>
       <c r="Q46" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="R46" t="str">
+        <v/>
+      </c>
+      <c r="S46" t="str">
         <v>C</v>
       </c>
-      <c r="S46" t="str">
+      <c r="T46" t="str">
         <v>D</v>
       </c>
-      <c r="T46" t="str">
+      <c r="U46" t="str">
+        <v/>
+      </c>
+      <c r="V46" t="str">
         <v>F</v>
-      </c>
-      <c r="U46" t="str">
-        <v/>
-      </c>
-      <c r="V46" t="str">
-        <v/>
       </c>
       <c r="X46" t="str">
         <v>B, C, D, F</v>
@@ -3374,22 +3392,22 @@
         <v>James, Patricia, Jennifer</v>
       </c>
       <c r="Q47" t="str">
+        <v/>
+      </c>
+      <c r="R47" t="str">
         <v>B</v>
       </c>
-      <c r="R47" t="str">
+      <c r="S47" t="str">
         <v>C</v>
       </c>
-      <c r="S47" t="str">
-        <v>E</v>
-      </c>
       <c r="T47" t="str">
+        <v>D</v>
+      </c>
+      <c r="U47" t="str">
+        <v/>
+      </c>
+      <c r="V47" t="str">
         <v>F</v>
-      </c>
-      <c r="U47" t="str">
-        <v/>
-      </c>
-      <c r="V47" t="str">
-        <v/>
       </c>
       <c r="X47" t="str">
         <v>B, C, E, F</v>
@@ -3418,22 +3436,22 @@
         <v>James, John</v>
       </c>
       <c r="Q48" t="str">
+        <v>A</v>
+      </c>
+      <c r="R48" t="str">
         <v>B</v>
       </c>
-      <c r="R48" t="str">
+      <c r="S48" t="str">
+        <v>C</v>
+      </c>
+      <c r="T48" t="str">
         <v>D</v>
       </c>
-      <c r="S48" t="str">
-        <v>E</v>
-      </c>
-      <c r="T48" t="str">
+      <c r="U48" t="str">
+        <v/>
+      </c>
+      <c r="V48" t="str">
         <v>F</v>
-      </c>
-      <c r="U48" t="str">
-        <v/>
-      </c>
-      <c r="V48" t="str">
-        <v/>
       </c>
       <c r="X48" t="str">
         <v>B, D, E, F</v>
@@ -3462,22 +3480,22 @@
         <v>James, John, Jennifer</v>
       </c>
       <c r="Q49" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="R49" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="S49" t="str">
-        <v>D</v>
+        <v/>
       </c>
       <c r="T49" t="str">
+        <v/>
+      </c>
+      <c r="U49" t="str">
         <v>E</v>
       </c>
-      <c r="U49" t="str">
+      <c r="V49" t="str">
         <v>F</v>
-      </c>
-      <c r="V49" t="str">
-        <v/>
       </c>
       <c r="X49" t="str">
         <v>B, C, D, E, F</v>
@@ -3506,7 +3524,7 @@
         <v>James, Jennifer</v>
       </c>
       <c r="Q50" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="R50" t="str">
         <v/>
@@ -3518,10 +3536,10 @@
         <v/>
       </c>
       <c r="U50" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V50" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X50" t="str">
         <v>C</v>
@@ -3550,10 +3568,10 @@
         <v>Robert</v>
       </c>
       <c r="Q51" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="R51" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="S51" t="str">
         <v/>
@@ -3562,10 +3580,10 @@
         <v/>
       </c>
       <c r="U51" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V51" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X51" t="str">
         <v>C, D</v>
@@ -3594,22 +3612,22 @@
         <v>Robert, Patricia</v>
       </c>
       <c r="Q52" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="R52" t="str">
+        <v>B</v>
+      </c>
+      <c r="S52" t="str">
+        <v/>
+      </c>
+      <c r="T52" t="str">
+        <v/>
+      </c>
+      <c r="U52" t="str">
         <v>E</v>
       </c>
-      <c r="S52" t="str">
-        <v/>
-      </c>
-      <c r="T52" t="str">
-        <v/>
-      </c>
-      <c r="U52" t="str">
-        <v/>
-      </c>
       <c r="V52" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X52" t="str">
         <v>C, E</v>
@@ -3638,22 +3656,22 @@
         <v>Robert, Patricia, John</v>
       </c>
       <c r="Q53" t="str">
+        <v/>
+      </c>
+      <c r="R53" t="str">
+        <v/>
+      </c>
+      <c r="S53" t="str">
         <v>C</v>
       </c>
-      <c r="R53" t="str">
+      <c r="T53" t="str">
+        <v/>
+      </c>
+      <c r="U53" t="str">
+        <v>E</v>
+      </c>
+      <c r="V53" t="str">
         <v>F</v>
-      </c>
-      <c r="S53" t="str">
-        <v/>
-      </c>
-      <c r="T53" t="str">
-        <v/>
-      </c>
-      <c r="U53" t="str">
-        <v/>
-      </c>
-      <c r="V53" t="str">
-        <v/>
       </c>
       <c r="X53" t="str">
         <v>C, F</v>
@@ -3682,22 +3700,22 @@
         <v>Robert, Patricia, John, Jennifer</v>
       </c>
       <c r="Q54" t="str">
+        <v>A</v>
+      </c>
+      <c r="R54" t="str">
+        <v/>
+      </c>
+      <c r="S54" t="str">
         <v>C</v>
       </c>
-      <c r="R54" t="str">
-        <v>D</v>
-      </c>
-      <c r="S54" t="str">
+      <c r="T54" t="str">
+        <v/>
+      </c>
+      <c r="U54" t="str">
         <v>E</v>
       </c>
-      <c r="T54" t="str">
-        <v/>
-      </c>
-      <c r="U54" t="str">
-        <v/>
-      </c>
       <c r="V54" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X54" t="str">
         <v>C, D, E</v>
@@ -3726,22 +3744,22 @@
         <v>Robert, Patricia, Jennifer</v>
       </c>
       <c r="Q55" t="str">
+        <v/>
+      </c>
+      <c r="R55" t="str">
+        <v>B</v>
+      </c>
+      <c r="S55" t="str">
         <v>C</v>
       </c>
-      <c r="R55" t="str">
-        <v>D</v>
-      </c>
-      <c r="S55" t="str">
+      <c r="T55" t="str">
+        <v/>
+      </c>
+      <c r="U55" t="str">
+        <v>E</v>
+      </c>
+      <c r="V55" t="str">
         <v>F</v>
-      </c>
-      <c r="T55" t="str">
-        <v/>
-      </c>
-      <c r="U55" t="str">
-        <v/>
-      </c>
-      <c r="V55" t="str">
-        <v/>
       </c>
       <c r="X55" t="str">
         <v>C, D, F</v>
@@ -3770,22 +3788,22 @@
         <v>Robert, John</v>
       </c>
       <c r="Q56" t="str">
+        <v>A</v>
+      </c>
+      <c r="R56" t="str">
+        <v>B</v>
+      </c>
+      <c r="S56" t="str">
         <v>C</v>
       </c>
-      <c r="R56" t="str">
+      <c r="T56" t="str">
+        <v/>
+      </c>
+      <c r="U56" t="str">
         <v>E</v>
       </c>
-      <c r="S56" t="str">
+      <c r="V56" t="str">
         <v>F</v>
-      </c>
-      <c r="T56" t="str">
-        <v/>
-      </c>
-      <c r="U56" t="str">
-        <v/>
-      </c>
-      <c r="V56" t="str">
-        <v/>
       </c>
       <c r="X56" t="str">
         <v>C, E, F</v>
@@ -3814,22 +3832,22 @@
         <v>Robert, John, Jennifer</v>
       </c>
       <c r="Q57" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="R57" t="str">
+        <v/>
+      </c>
+      <c r="S57" t="str">
+        <v/>
+      </c>
+      <c r="T57" t="str">
         <v>D</v>
       </c>
-      <c r="S57" t="str">
+      <c r="U57" t="str">
         <v>E</v>
       </c>
-      <c r="T57" t="str">
+      <c r="V57" t="str">
         <v>F</v>
-      </c>
-      <c r="U57" t="str">
-        <v/>
-      </c>
-      <c r="V57" t="str">
-        <v/>
       </c>
       <c r="X57" t="str">
         <v>C, D, E, F</v>
@@ -3858,22 +3876,22 @@
         <v>Robert, Jennifer</v>
       </c>
       <c r="Q58" t="str">
+        <v>A</v>
+      </c>
+      <c r="R58" t="str">
+        <v/>
+      </c>
+      <c r="S58" t="str">
+        <v/>
+      </c>
+      <c r="T58" t="str">
         <v>D</v>
       </c>
-      <c r="R58" t="str">
-        <v/>
-      </c>
-      <c r="S58" t="str">
-        <v/>
-      </c>
-      <c r="T58" t="str">
-        <v/>
-      </c>
       <c r="U58" t="str">
-        <v/>
+        <v>E</v>
       </c>
       <c r="V58" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X58" t="str">
         <v>D</v>
@@ -3902,22 +3920,22 @@
         <v>Patricia</v>
       </c>
       <c r="Q59" t="str">
+        <v/>
+      </c>
+      <c r="R59" t="str">
+        <v>B</v>
+      </c>
+      <c r="S59" t="str">
+        <v/>
+      </c>
+      <c r="T59" t="str">
         <v>D</v>
       </c>
-      <c r="R59" t="str">
+      <c r="U59" t="str">
         <v>E</v>
       </c>
-      <c r="S59" t="str">
-        <v/>
-      </c>
-      <c r="T59" t="str">
-        <v/>
-      </c>
-      <c r="U59" t="str">
-        <v/>
-      </c>
       <c r="V59" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X59" t="str">
         <v>D, E</v>
@@ -3946,22 +3964,22 @@
         <v>Patricia, John</v>
       </c>
       <c r="Q60" t="str">
+        <v>A</v>
+      </c>
+      <c r="R60" t="str">
+        <v>B</v>
+      </c>
+      <c r="S60" t="str">
+        <v/>
+      </c>
+      <c r="T60" t="str">
         <v>D</v>
       </c>
-      <c r="R60" t="str">
+      <c r="U60" t="str">
+        <v>E</v>
+      </c>
+      <c r="V60" t="str">
         <v>F</v>
-      </c>
-      <c r="S60" t="str">
-        <v/>
-      </c>
-      <c r="T60" t="str">
-        <v/>
-      </c>
-      <c r="U60" t="str">
-        <v/>
-      </c>
-      <c r="V60" t="str">
-        <v/>
       </c>
       <c r="X60" t="str">
         <v>D, F</v>
@@ -3990,22 +4008,22 @@
         <v>Patricia, John, Jennifer</v>
       </c>
       <c r="Q61" t="str">
+        <v/>
+      </c>
+      <c r="R61" t="str">
+        <v/>
+      </c>
+      <c r="S61" t="str">
+        <v>C</v>
+      </c>
+      <c r="T61" t="str">
         <v>D</v>
       </c>
-      <c r="R61" t="str">
+      <c r="U61" t="str">
         <v>E</v>
       </c>
-      <c r="S61" t="str">
+      <c r="V61" t="str">
         <v>F</v>
-      </c>
-      <c r="T61" t="str">
-        <v/>
-      </c>
-      <c r="U61" t="str">
-        <v/>
-      </c>
-      <c r="V61" t="str">
-        <v/>
       </c>
       <c r="X61" t="str">
         <v>D, E, F</v>
@@ -4034,22 +4052,22 @@
         <v>Patricia, Jennifer</v>
       </c>
       <c r="Q62" t="str">
+        <v>A</v>
+      </c>
+      <c r="R62" t="str">
+        <v/>
+      </c>
+      <c r="S62" t="str">
+        <v>C</v>
+      </c>
+      <c r="T62" t="str">
+        <v>D</v>
+      </c>
+      <c r="U62" t="str">
         <v>E</v>
       </c>
-      <c r="R62" t="str">
-        <v/>
-      </c>
-      <c r="S62" t="str">
-        <v/>
-      </c>
-      <c r="T62" t="str">
-        <v/>
-      </c>
-      <c r="U62" t="str">
-        <v/>
-      </c>
       <c r="V62" t="str">
-        <v/>
+        <v>F</v>
       </c>
       <c r="X62" t="str">
         <v>E</v>
@@ -4078,22 +4096,22 @@
         <v>John</v>
       </c>
       <c r="Q63" t="str">
+        <v/>
+      </c>
+      <c r="R63" t="str">
+        <v>B</v>
+      </c>
+      <c r="S63" t="str">
+        <v>C</v>
+      </c>
+      <c r="T63" t="str">
+        <v>D</v>
+      </c>
+      <c r="U63" t="str">
         <v>E</v>
       </c>
-      <c r="R63" t="str">
+      <c r="V63" t="str">
         <v>F</v>
-      </c>
-      <c r="S63" t="str">
-        <v/>
-      </c>
-      <c r="T63" t="str">
-        <v/>
-      </c>
-      <c r="U63" t="str">
-        <v/>
-      </c>
-      <c r="V63" t="str">
-        <v/>
       </c>
       <c r="X63" t="str">
         <v>E, F</v>
@@ -4122,22 +4140,22 @@
         <v>John, Jennifer</v>
       </c>
       <c r="Q64" t="str">
+        <v>A</v>
+      </c>
+      <c r="R64" t="str">
+        <v>B</v>
+      </c>
+      <c r="S64" t="str">
+        <v>C</v>
+      </c>
+      <c r="T64" t="str">
+        <v>D</v>
+      </c>
+      <c r="U64" t="str">
+        <v>E</v>
+      </c>
+      <c r="V64" t="str">
         <v>F</v>
-      </c>
-      <c r="R64" t="str">
-        <v/>
-      </c>
-      <c r="S64" t="str">
-        <v/>
-      </c>
-      <c r="T64" t="str">
-        <v/>
-      </c>
-      <c r="U64" t="str">
-        <v/>
-      </c>
-      <c r="V64" t="str">
-        <v/>
       </c>
       <c r="X64" t="str">
         <v>F</v>
@@ -4163,10 +4181,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8245AC4-F41E-4164-B861-232B6B4759C3}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4182,7 +4200,7 @@
     <col min="10" max="11" width="39.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4211,8 +4229,16 @@
       <c r="K1" t="str">
         <v>James</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M1" s="14" t="str" cm="1">
+        <f t="array" ref="M1:N64">_xlfn.LET(_xlpm.r,A2:A7,_xlpm.i,_xlfn.LAMBDA(_xlpm.x,_xlfn.DROP(_xlfn.TEXTAFTER(_xlfn.REDUCE("",_xlpm.x,_xlfn.LAMBDA(_xlpm.a,_xlpm.d,_xlfn.VSTACK(_xlpm.a,_xlpm.a&amp;", "&amp;_xlpm.d))),", "),1)),
+_xlpm.v,_xlpm.i(_xlpm.r),_xlfn.VSTACK(A1:B1,_xlfn.SORTBY(_xlfn.HSTACK(_xlpm.v,_xlpm.i(B2:B7)),LEN(_xlpm.v),,_xlfn.XMATCH(LEFT(_xlpm.v),_xlfn.VSTACK(_xlpm.r,_xlfn.DROP(CHAR(_xlfn.SEQUENCE(26)+64),ROWS(_xlpm.r)))),)))</f>
+        <v>Dept</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Name</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -4237,8 +4263,14 @@
       <c r="K2" t="str">
         <v>Mary</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M2" t="str">
+        <v>B</v>
+      </c>
+      <c r="N2" t="str">
+        <v>James</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4263,8 +4295,14 @@
       <c r="K3" t="str">
         <v>Robert,X</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M3" t="str">
+        <v>A</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Mary</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -4289,8 +4327,14 @@
       <c r="K4" t="str">
         <v>Patricia</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M4" t="str">
+        <v>D</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Robert,X</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -4315,8 +4359,14 @@
       <c r="K5" t="str">
         <v>John</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M5" t="str">
+        <v>C</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Patricia</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -4341,8 +4391,14 @@
       <c r="K6" t="str">
         <v>Jennifer</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M6" t="str">
+        <v>E</v>
+      </c>
+      <c r="N6" t="str">
+        <v>John</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -4367,8 +4423,14 @@
       <c r="K7" t="str">
         <v>James, Mary</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M7" t="str">
+        <v>F</v>
+      </c>
+      <c r="N7" t="str">
+        <v>Jennifer</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="str">
         <v>B, A</v>
       </c>
@@ -4387,8 +4449,14 @@
       <c r="K8" t="str">
         <v>James, Robert,X</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M8" t="str">
+        <v>B, A</v>
+      </c>
+      <c r="N8" t="str">
+        <v>James, Mary</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D9" s="7" t="str">
         <v>B, D</v>
       </c>
@@ -4407,8 +4475,14 @@
       <c r="K9" t="str">
         <v>James, Patricia</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M9" t="str">
+        <v>B, D</v>
+      </c>
+      <c r="N9" t="str">
+        <v>James, Robert,X</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D10" s="7" t="str">
         <v>A, D</v>
       </c>
@@ -4427,8 +4501,14 @@
       <c r="K10" t="str">
         <v>James, John</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M10" t="str">
+        <v>B, C</v>
+      </c>
+      <c r="N10" t="str">
+        <v>James, Patricia</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D11" s="7" t="str">
         <v>B, C</v>
       </c>
@@ -4447,8 +4527,14 @@
       <c r="K11" t="str">
         <v>James, Jennifer</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M11" t="str">
+        <v>B, E</v>
+      </c>
+      <c r="N11" t="str">
+        <v>James, John</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D12" s="7" t="str">
         <v>A, C</v>
       </c>
@@ -4467,8 +4553,14 @@
       <c r="K12" t="str">
         <v>Mary, Robert,X</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M12" t="str">
+        <v>B, F</v>
+      </c>
+      <c r="N12" t="str">
+        <v>James, Jennifer</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D13" s="7" t="str">
         <v>D, C</v>
       </c>
@@ -4487,8 +4579,14 @@
       <c r="K13" t="str">
         <v>Mary, Patricia</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M13" t="str">
+        <v>A, D</v>
+      </c>
+      <c r="N13" t="str">
+        <v>Mary, Robert,X</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" s="7" t="str">
         <v>B, E</v>
       </c>
@@ -4507,8 +4605,14 @@
       <c r="K14" t="str">
         <v>Mary, John</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M14" t="str">
+        <v>A, C</v>
+      </c>
+      <c r="N14" t="str">
+        <v>Mary, Patricia</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D15" s="7" t="str">
         <v>A, E</v>
       </c>
@@ -4527,8 +4631,14 @@
       <c r="K15" t="str">
         <v>Mary, Jennifer</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M15" t="str">
+        <v>A, E</v>
+      </c>
+      <c r="N15" t="str">
+        <v>Mary, John</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D16" s="7" t="str">
         <v>D, E</v>
       </c>
@@ -4547,8 +4657,14 @@
       <c r="K16" t="str">
         <v>Robert,X, Patricia</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M16" t="str">
+        <v>A, F</v>
+      </c>
+      <c r="N16" t="str">
+        <v>Mary, Jennifer</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D17" s="7" t="str">
         <v>C, E</v>
       </c>
@@ -4567,8 +4683,14 @@
       <c r="K17" t="str">
         <v>Robert,X, John</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M17" t="str">
+        <v>D, C</v>
+      </c>
+      <c r="N17" t="str">
+        <v>Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D18" s="7" t="str">
         <v>B, F</v>
       </c>
@@ -4587,8 +4709,14 @@
       <c r="K18" t="str">
         <v>Robert,X, Jennifer</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M18" t="str">
+        <v>D, E</v>
+      </c>
+      <c r="N18" t="str">
+        <v>Robert,X, John</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D19" s="7" t="str">
         <v>A, F</v>
       </c>
@@ -4607,8 +4735,14 @@
       <c r="K19" t="str">
         <v>Patricia, John</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M19" t="str">
+        <v>D, F</v>
+      </c>
+      <c r="N19" t="str">
+        <v>Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D20" s="7" t="str">
         <v>D, F</v>
       </c>
@@ -4627,8 +4761,14 @@
       <c r="K20" t="str">
         <v>Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M20" t="str">
+        <v>C, E</v>
+      </c>
+      <c r="N20" t="str">
+        <v>Patricia, John</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D21" s="7" t="str">
         <v>C, F</v>
       </c>
@@ -4647,8 +4787,14 @@
       <c r="K21" t="str">
         <v>John, Jennifer</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M21" t="str">
+        <v>C, F</v>
+      </c>
+      <c r="N21" t="str">
+        <v>Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D22" s="7" t="str">
         <v>E, F</v>
       </c>
@@ -4667,8 +4813,14 @@
       <c r="K22" t="str">
         <v>James, Mary, Robert,X</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M22" t="str">
+        <v>E, F</v>
+      </c>
+      <c r="N22" t="str">
+        <v>John, Jennifer</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D23" s="7" t="str">
         <v>B, A, D</v>
       </c>
@@ -4687,8 +4839,14 @@
       <c r="K23" t="str">
         <v>James, Mary, Patricia</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M23" t="str">
+        <v>B, A, D</v>
+      </c>
+      <c r="N23" t="str">
+        <v>James, Mary, Robert,X</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D24" s="7" t="str">
         <v>B, A, C</v>
       </c>
@@ -4707,8 +4865,14 @@
       <c r="K24" t="str">
         <v>James, Mary, John</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M24" t="str">
+        <v>B, A, C</v>
+      </c>
+      <c r="N24" t="str">
+        <v>James, Mary, Patricia</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D25" s="7" t="str">
         <v>B, D, C</v>
       </c>
@@ -4727,8 +4891,14 @@
       <c r="K25" t="str">
         <v>James, Mary, Jennifer</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M25" s="15" t="str">
+        <v>B, D, C</v>
+      </c>
+      <c r="N25" t="str">
+        <v>James, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D26" s="7" t="str">
         <v>A, D, C</v>
       </c>
@@ -4747,8 +4917,14 @@
       <c r="K26" t="str">
         <v>James, Robert,X, Patricia</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M26" s="15" t="str">
+        <v>B, A, E</v>
+      </c>
+      <c r="N26" t="str">
+        <v>James, Mary, John</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D27" s="7" t="str">
         <v>B, A, E</v>
       </c>
@@ -4767,8 +4943,14 @@
       <c r="K27" t="str">
         <v>James, Robert,X, John</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M27" t="str">
+        <v>B, D, E</v>
+      </c>
+      <c r="N27" t="str">
+        <v>James, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D28" s="7" t="str">
         <v>B, D, E</v>
       </c>
@@ -4787,8 +4969,14 @@
       <c r="K28" t="str">
         <v>James, Robert,X, Jennifer</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M28" t="str">
+        <v>B, C, E</v>
+      </c>
+      <c r="N28" t="str">
+        <v>James, Patricia, John</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D29" s="7" t="str">
         <v>A, D, E</v>
       </c>
@@ -4807,8 +4995,14 @@
       <c r="K29" t="str">
         <v>James, Patricia, John</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M29" t="str">
+        <v>B, A, F</v>
+      </c>
+      <c r="N29" t="str">
+        <v>James, Mary, Jennifer</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D30" s="7" t="str">
         <v>B, C, E</v>
       </c>
@@ -4827,8 +5021,14 @@
       <c r="K30" t="str">
         <v>James, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M30" t="str">
+        <v>B, D, F</v>
+      </c>
+      <c r="N30" t="str">
+        <v>James, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D31" s="7" t="str">
         <v>A, C, E</v>
       </c>
@@ -4847,8 +5047,14 @@
       <c r="K31" t="str">
         <v>James, John, Jennifer</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M31" t="str">
+        <v>B, C, F</v>
+      </c>
+      <c r="N31" t="str">
+        <v>James, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D32" s="7" t="str">
         <v>D, C, E</v>
       </c>
@@ -4867,8 +5073,14 @@
       <c r="K32" t="str">
         <v>Mary, Robert,X, Patricia</v>
       </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M32" t="str">
+        <v>B, E, F</v>
+      </c>
+      <c r="N32" t="str">
+        <v>James, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D33" s="7" t="str">
         <v>B, A, F</v>
       </c>
@@ -4887,8 +5099,14 @@
       <c r="K33" t="str">
         <v>Mary, Robert,X, John</v>
       </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M33" t="str">
+        <v>A, D, C</v>
+      </c>
+      <c r="N33" t="str">
+        <v>Mary, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D34" s="7" t="str">
         <v>B, D, F</v>
       </c>
@@ -4907,8 +5125,14 @@
       <c r="K34" t="str">
         <v>Mary, Robert,X, Jennifer</v>
       </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M34" t="str">
+        <v>A, D, E</v>
+      </c>
+      <c r="N34" t="str">
+        <v>Mary, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D35" s="7" t="str">
         <v>A, D, F</v>
       </c>
@@ -4927,8 +5151,14 @@
       <c r="K35" t="str">
         <v>Mary, Patricia, John</v>
       </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M35" t="str">
+        <v>A, C, E</v>
+      </c>
+      <c r="N35" t="str">
+        <v>Mary, Patricia, John</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D36" s="7" t="str">
         <v>B, C, F</v>
       </c>
@@ -4947,8 +5177,14 @@
       <c r="K36" t="str">
         <v>Mary, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M36" t="str">
+        <v>A, D, F</v>
+      </c>
+      <c r="N36" t="str">
+        <v>Mary, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D37" s="7" t="str">
         <v>A, C, F</v>
       </c>
@@ -4967,8 +5203,14 @@
       <c r="K37" t="str">
         <v>Mary, John, Jennifer</v>
       </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M37" t="str">
+        <v>A, C, F</v>
+      </c>
+      <c r="N37" t="str">
+        <v>Mary, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D38" s="7" t="str">
         <v>D, C, F</v>
       </c>
@@ -4987,8 +5229,14 @@
       <c r="K38" t="str">
         <v>Robert,X, Patricia, John</v>
       </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M38" t="str">
+        <v>A, E, F</v>
+      </c>
+      <c r="N38" t="str">
+        <v>Mary, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D39" s="7" t="str">
         <v>B, E, F</v>
       </c>
@@ -5007,8 +5255,14 @@
       <c r="K39" t="str">
         <v>Robert,X, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M39" t="str">
+        <v>D, C, E</v>
+      </c>
+      <c r="N39" t="str">
+        <v>Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D40" s="7" t="str">
         <v>A, E, F</v>
       </c>
@@ -5027,8 +5281,14 @@
       <c r="K40" t="str">
         <v>Robert,X, John, Jennifer</v>
       </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M40" t="str">
+        <v>D, C, F</v>
+      </c>
+      <c r="N40" t="str">
+        <v>Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D41" s="7" t="str">
         <v>D, E, F</v>
       </c>
@@ -5047,8 +5307,14 @@
       <c r="K41" t="str">
         <v>Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M41" t="str">
+        <v>D, E, F</v>
+      </c>
+      <c r="N41" t="str">
+        <v>Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D42" s="7" t="str">
         <v>C, E, F</v>
       </c>
@@ -5067,8 +5333,14 @@
       <c r="K42" t="str">
         <v>James, Mary, Robert,X, Patricia</v>
       </c>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M42" t="str">
+        <v>C, E, F</v>
+      </c>
+      <c r="N42" t="str">
+        <v>Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D43" s="7" t="str">
         <v>B, A, D, C</v>
       </c>
@@ -5087,8 +5359,14 @@
       <c r="K43" t="str">
         <v>James, Mary, Robert,X, John</v>
       </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M43" t="str">
+        <v>B, A, D, C</v>
+      </c>
+      <c r="N43" t="str">
+        <v>James, Mary, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D44" s="7" t="str">
         <v>B, A, D, E</v>
       </c>
@@ -5107,8 +5385,14 @@
       <c r="K44" t="str">
         <v>James, Mary, Robert,X, Jennifer</v>
       </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M44" t="str">
+        <v>B, A, D, E</v>
+      </c>
+      <c r="N44" t="str">
+        <v>James, Mary, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D45" s="7" t="str">
         <v>B, A, C, E</v>
       </c>
@@ -5127,8 +5411,14 @@
       <c r="K45" t="str">
         <v>James, Mary, Patricia, John</v>
       </c>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M45" t="str">
+        <v>B, A, C, E</v>
+      </c>
+      <c r="N45" t="str">
+        <v>James, Mary, Patricia, John</v>
+      </c>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D46" s="7" t="str">
         <v>B, D, C, E</v>
       </c>
@@ -5147,8 +5437,14 @@
       <c r="K46" t="str">
         <v>James, Mary, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M46" t="str">
+        <v>B, D, C, E</v>
+      </c>
+      <c r="N46" t="str">
+        <v>James, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="47" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D47" s="7" t="str">
         <v>A, D, C, E</v>
       </c>
@@ -5167,8 +5463,14 @@
       <c r="K47" t="str">
         <v>James, Mary, John, Jennifer</v>
       </c>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M47" t="str">
+        <v>B, A, D, F</v>
+      </c>
+      <c r="N47" t="str">
+        <v>James, Mary, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="48" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D48" s="7" t="str">
         <v>B, A, D, F</v>
       </c>
@@ -5187,8 +5489,14 @@
       <c r="K48" t="str">
         <v>James, Robert,X, Patricia, John</v>
       </c>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M48" t="str">
+        <v>B, A, C, F</v>
+      </c>
+      <c r="N48" t="str">
+        <v>James, Mary, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D49" s="7" t="str">
         <v>B, A, C, F</v>
       </c>
@@ -5207,8 +5515,14 @@
       <c r="K49" t="str">
         <v>James, Robert,X, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M49" t="str">
+        <v>B, D, C, F</v>
+      </c>
+      <c r="N49" t="str">
+        <v>James, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D50" s="7" t="str">
         <v>B, D, C, F</v>
       </c>
@@ -5227,8 +5541,14 @@
       <c r="K50" t="str">
         <v>James, Robert,X, John, Jennifer</v>
       </c>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M50" t="str">
+        <v>B, A, E, F</v>
+      </c>
+      <c r="N50" t="str">
+        <v>James, Mary, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="51" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D51" s="7" t="str">
         <v>A, D, C, F</v>
       </c>
@@ -5247,8 +5567,14 @@
       <c r="K51" t="str">
         <v>James, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M51" t="str">
+        <v>B, D, E, F</v>
+      </c>
+      <c r="N51" t="str">
+        <v>James, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="52" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D52" s="7" t="str">
         <v>B, A, E, F</v>
       </c>
@@ -5267,8 +5593,14 @@
       <c r="K52" t="str">
         <v>Mary, Robert,X, Patricia, John</v>
       </c>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M52" t="str">
+        <v>B, C, E, F</v>
+      </c>
+      <c r="N52" t="str">
+        <v>James, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D53" s="7" t="str">
         <v>B, D, E, F</v>
       </c>
@@ -5287,8 +5619,14 @@
       <c r="K53" t="str">
         <v>Mary, Robert,X, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M53" t="str">
+        <v>A, D, C, E</v>
+      </c>
+      <c r="N53" t="str">
+        <v>Mary, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D54" s="7" t="str">
         <v>A, D, E, F</v>
       </c>
@@ -5307,8 +5645,14 @@
       <c r="K54" t="str">
         <v>Mary, Robert,X, John, Jennifer</v>
       </c>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M54" t="str">
+        <v>A, D, C, F</v>
+      </c>
+      <c r="N54" t="str">
+        <v>Mary, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="55" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D55" s="7" t="str">
         <v>B, C, E, F</v>
       </c>
@@ -5327,8 +5671,14 @@
       <c r="K55" t="str">
         <v>Mary, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M55" t="str">
+        <v>A, D, E, F</v>
+      </c>
+      <c r="N55" t="str">
+        <v>Mary, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="56" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D56" s="7" t="str">
         <v>A, C, E, F</v>
       </c>
@@ -5347,8 +5697,14 @@
       <c r="K56" t="str">
         <v>Robert,X, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M56" t="str">
+        <v>A, C, E, F</v>
+      </c>
+      <c r="N56" t="str">
+        <v>Mary, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="57" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D57" s="7" t="str">
         <v>D, C, E, F</v>
       </c>
@@ -5367,8 +5723,14 @@
       <c r="K57" t="str">
         <v>James, Mary, Robert,X, Patricia, John</v>
       </c>
-    </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M57" t="str">
+        <v>D, C, E, F</v>
+      </c>
+      <c r="N57" t="str">
+        <v>Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D58" s="7" t="str">
         <v>B, A, D, C, E</v>
       </c>
@@ -5387,8 +5749,14 @@
       <c r="K58" t="str">
         <v>James, Mary, Robert,X, Patricia, Jennifer</v>
       </c>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M58" t="str">
+        <v>B, A, D, C, E</v>
+      </c>
+      <c r="N58" t="str">
+        <v>James, Mary, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="59" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D59" s="7" t="str">
         <v>B, A, D, C, F</v>
       </c>
@@ -5407,8 +5775,14 @@
       <c r="K59" t="str">
         <v>James, Mary, Robert,X, John, Jennifer</v>
       </c>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M59" t="str">
+        <v>B, A, D, C, F</v>
+      </c>
+      <c r="N59" t="str">
+        <v>James, Mary, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="60" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D60" s="7" t="str">
         <v>B, A, D, E, F</v>
       </c>
@@ -5427,8 +5801,14 @@
       <c r="K60" t="str">
         <v>James, Mary, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M60" t="str">
+        <v>B, A, D, E, F</v>
+      </c>
+      <c r="N60" t="str">
+        <v>James, Mary, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="61" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D61" s="7" t="str">
         <v>B, A, C, E, F</v>
       </c>
@@ -5447,8 +5827,14 @@
       <c r="K61" t="str">
         <v>James, Robert,X, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M61" t="str">
+        <v>B, A, C, E, F</v>
+      </c>
+      <c r="N61" t="str">
+        <v>James, Mary, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="62" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D62" s="7" t="str">
         <v>B, D, C, E, F</v>
       </c>
@@ -5467,8 +5853,14 @@
       <c r="K62" t="str">
         <v>Mary, Robert,X, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M62" t="str">
+        <v>B, D, C, E, F</v>
+      </c>
+      <c r="N62" t="str">
+        <v>James, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="63" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D63" s="7" t="str">
         <v>A, D, C, E, F</v>
       </c>
@@ -5487,8 +5879,14 @@
       <c r="K63" t="str">
         <v>James, Mary, Robert,X, Patricia, John, Jennifer</v>
       </c>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="M63" t="str">
+        <v>A, D, C, E, F</v>
+      </c>
+      <c r="N63" t="str">
+        <v>Mary, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="64" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D64" s="11" t="str">
         <v>B, A, D, C, E, F</v>
       </c>
@@ -5499,6 +5897,587 @@
         <v>B, A, D, C, E, F</v>
       </c>
       <c r="H64" t="str">
+        <v>James, Mary, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+      <c r="M64" t="str">
+        <v>B, A, D, C, E, F</v>
+      </c>
+      <c r="N64" t="str">
+        <v>James, Mary, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075835FD-3E5C-4E86-9499-6A63A755A9FA}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="K2:O65"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="str" cm="1">
+        <f t="array" ref="N2:O65">_xlfn.LET(_xlpm.DeptData, K3:K8, _xlpm.Header, K2:L2, _xlpm.PatternGen, _xlfn.LAMBDA(_xlpm.Vector, _xlfn.DROP(_xlfn.TEXTAFTER(_xlfn.REDUCE("", _xlpm.Vector, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.VSTACK(_xlpm.Acc, _xlpm.Acc &amp; ", " &amp; _xlpm.Curr))), ", "), 1)), _xlpm.DeptPattern, _xlpm.PatternGen(_xlpm.DeptData), _xlpm.NamePattern, _xlpm.PatternGen(L3:L8), _xlpm.AllPatternStack, _xlfn.HSTACK(_xlpm.DeptPattern, _xlpm.NamePattern), _xlpm.y, _xlfn.LAMBDA(_xlpm.x, _xlfn.XMATCH(MID(_xlpm.DeptPattern, _xlpm.x, 1), _xlfn.TAKE(_xlfn.VSTACK(_xlpm.DeptData, CHAR(_xlfn.SEQUENCE(26) + 64)), 26))), _xlpm._Y1, _xlpm.y(1), _xlpm._Y4, _xlpm.y(4), _xlpm._Y7, _xlpm.y(7), _xlpm.Result, _xlfn.VSTACK(_xlpm.Header, _xlfn.SORTBY(_xlpm.AllPatternStack, LEN(_xlpm.DeptPattern), , _xlpm._Y1, , _xlpm._Y4, , _xlpm._Y7, )), _xlpm.Result)</f>
+        <v>Dept</v>
+      </c>
+      <c r="O2" t="str">
+        <v>Name</v>
+      </c>
+    </row>
+    <row r="3" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="str">
+        <v>B</v>
+      </c>
+      <c r="O3" t="str">
+        <v>James</v>
+      </c>
+    </row>
+    <row r="4" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="str">
+        <v>D</v>
+      </c>
+      <c r="O4" t="str">
+        <v>Robert,X</v>
+      </c>
+    </row>
+    <row r="5" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" t="str">
+        <v>C</v>
+      </c>
+      <c r="O5" t="str">
+        <v>Patricia</v>
+      </c>
+    </row>
+    <row r="6" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" t="str">
+        <v>E</v>
+      </c>
+      <c r="O6" t="str">
+        <v>John</v>
+      </c>
+    </row>
+    <row r="7" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="str">
+        <v>F</v>
+      </c>
+      <c r="O7" t="str">
+        <v>Jennifer</v>
+      </c>
+    </row>
+    <row r="8" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="str">
+        <v>AX</v>
+      </c>
+      <c r="O8" t="str">
+        <v>Mary</v>
+      </c>
+    </row>
+    <row r="9" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N9" t="str">
+        <v>B, D</v>
+      </c>
+      <c r="O9" t="str">
+        <v>James, Robert,X</v>
+      </c>
+    </row>
+    <row r="10" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N10" t="str">
+        <v>B, C</v>
+      </c>
+      <c r="O10" t="str">
+        <v>James, Patricia</v>
+      </c>
+    </row>
+    <row r="11" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N11" t="str">
+        <v>B, E</v>
+      </c>
+      <c r="O11" t="str">
+        <v>James, John</v>
+      </c>
+    </row>
+    <row r="12" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N12" t="str">
+        <v>B, F</v>
+      </c>
+      <c r="O12" t="str">
+        <v>James, Jennifer</v>
+      </c>
+    </row>
+    <row r="13" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N13" t="str">
+        <v>D, C</v>
+      </c>
+      <c r="O13" t="str">
+        <v>Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="14" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N14" t="str">
+        <v>D, E</v>
+      </c>
+      <c r="O14" t="str">
+        <v>Robert,X, John</v>
+      </c>
+    </row>
+    <row r="15" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N15" t="str">
+        <v>D, F</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="16" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="N16" t="str">
+        <v>C, E</v>
+      </c>
+      <c r="O16" t="str">
+        <v>Patricia, John</v>
+      </c>
+    </row>
+    <row r="17" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N17" t="str">
+        <v>C, F</v>
+      </c>
+      <c r="O17" t="str">
+        <v>Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="18" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N18" t="str">
+        <v>E, F</v>
+      </c>
+      <c r="O18" t="str">
+        <v>John, Jennifer</v>
+      </c>
+    </row>
+    <row r="19" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N19" t="str">
+        <v>B, AX</v>
+      </c>
+      <c r="O19" t="str">
+        <v>James, Mary</v>
+      </c>
+    </row>
+    <row r="20" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N20" t="str">
+        <v>AX, D</v>
+      </c>
+      <c r="O20" t="str">
+        <v>Mary, Robert,X</v>
+      </c>
+    </row>
+    <row r="21" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N21" t="str">
+        <v>AX, C</v>
+      </c>
+      <c r="O21" t="str">
+        <v>Mary, Patricia</v>
+      </c>
+    </row>
+    <row r="22" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N22" t="str">
+        <v>AX, E</v>
+      </c>
+      <c r="O22" t="str">
+        <v>Mary, John</v>
+      </c>
+    </row>
+    <row r="23" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N23" t="str">
+        <v>AX, F</v>
+      </c>
+      <c r="O23" t="str">
+        <v>Mary, Jennifer</v>
+      </c>
+    </row>
+    <row r="24" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N24" t="str">
+        <v>B, D, C</v>
+      </c>
+      <c r="O24" t="str">
+        <v>James, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="25" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N25" t="str">
+        <v>B, D, E</v>
+      </c>
+      <c r="O25" t="str">
+        <v>James, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="26" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N26" t="str">
+        <v>B, D, F</v>
+      </c>
+      <c r="O26" t="str">
+        <v>James, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="27" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N27" t="str">
+        <v>B, C, E</v>
+      </c>
+      <c r="O27" t="str">
+        <v>James, Patricia, John</v>
+      </c>
+    </row>
+    <row r="28" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N28" t="str">
+        <v>B, C, F</v>
+      </c>
+      <c r="O28" t="str">
+        <v>James, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="29" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N29" t="str">
+        <v>B, E, F</v>
+      </c>
+      <c r="O29" t="str">
+        <v>James, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="30" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N30" t="str">
+        <v>D, C, E</v>
+      </c>
+      <c r="O30" t="str">
+        <v>Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="31" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N31" t="str">
+        <v>D, C, F</v>
+      </c>
+      <c r="O31" t="str">
+        <v>Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="32" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N32" t="str">
+        <v>D, E, F</v>
+      </c>
+      <c r="O32" t="str">
+        <v>Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="33" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N33" t="str">
+        <v>C, E, F</v>
+      </c>
+      <c r="O33" t="str">
+        <v>Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="34" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N34" t="str">
+        <v>B, AX, D</v>
+      </c>
+      <c r="O34" t="str">
+        <v>James, Mary, Robert,X</v>
+      </c>
+    </row>
+    <row r="35" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N35" t="str">
+        <v>B, AX, C</v>
+      </c>
+      <c r="O35" t="str">
+        <v>James, Mary, Patricia</v>
+      </c>
+    </row>
+    <row r="36" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N36" t="str">
+        <v>B, AX, E</v>
+      </c>
+      <c r="O36" t="str">
+        <v>James, Mary, John</v>
+      </c>
+    </row>
+    <row r="37" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N37" t="str">
+        <v>B, AX, F</v>
+      </c>
+      <c r="O37" t="str">
+        <v>James, Mary, Jennifer</v>
+      </c>
+    </row>
+    <row r="38" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N38" t="str">
+        <v>AX, D, C</v>
+      </c>
+      <c r="O38" t="str">
+        <v>Mary, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="39" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N39" t="str">
+        <v>AX, D, E</v>
+      </c>
+      <c r="O39" t="str">
+        <v>Mary, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="40" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N40" t="str">
+        <v>AX, C, E</v>
+      </c>
+      <c r="O40" t="str">
+        <v>Mary, Patricia, John</v>
+      </c>
+    </row>
+    <row r="41" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N41" t="str">
+        <v>AX, D, F</v>
+      </c>
+      <c r="O41" t="str">
+        <v>Mary, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="42" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N42" t="str">
+        <v>AX, C, F</v>
+      </c>
+      <c r="O42" t="str">
+        <v>Mary, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="43" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N43" t="str">
+        <v>AX, E, F</v>
+      </c>
+      <c r="O43" t="str">
+        <v>Mary, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="44" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N44" t="str">
+        <v>B, D, C, E</v>
+      </c>
+      <c r="O44" t="str">
+        <v>James, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="45" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N45" t="str">
+        <v>B, D, C, F</v>
+      </c>
+      <c r="O45" t="str">
+        <v>James, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="46" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N46" t="str">
+        <v>B, D, E, F</v>
+      </c>
+      <c r="O46" t="str">
+        <v>James, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="47" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N47" t="str">
+        <v>B, C, E, F</v>
+      </c>
+      <c r="O47" t="str">
+        <v>James, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="48" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N48" t="str">
+        <v>D, C, E, F</v>
+      </c>
+      <c r="O48" t="str">
+        <v>Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="49" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N49" t="str">
+        <v>B, AX, D, C</v>
+      </c>
+      <c r="O49" t="str">
+        <v>James, Mary, Robert,X, Patricia</v>
+      </c>
+    </row>
+    <row r="50" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N50" t="str">
+        <v>B, AX, D, E</v>
+      </c>
+      <c r="O50" t="str">
+        <v>James, Mary, Robert,X, John</v>
+      </c>
+    </row>
+    <row r="51" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N51" t="str">
+        <v>B, AX, C, E</v>
+      </c>
+      <c r="O51" t="str">
+        <v>James, Mary, Patricia, John</v>
+      </c>
+    </row>
+    <row r="52" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N52" t="str">
+        <v>B, AX, D, F</v>
+      </c>
+      <c r="O52" t="str">
+        <v>James, Mary, Robert,X, Jennifer</v>
+      </c>
+    </row>
+    <row r="53" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N53" t="str">
+        <v>B, AX, C, F</v>
+      </c>
+      <c r="O53" t="str">
+        <v>James, Mary, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="54" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N54" t="str">
+        <v>B, AX, E, F</v>
+      </c>
+      <c r="O54" t="str">
+        <v>James, Mary, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="55" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N55" t="str">
+        <v>AX, D, C, E</v>
+      </c>
+      <c r="O55" t="str">
+        <v>Mary, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="56" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N56" t="str">
+        <v>AX, D, C, F</v>
+      </c>
+      <c r="O56" t="str">
+        <v>Mary, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="57" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N57" t="str">
+        <v>AX, D, E, F</v>
+      </c>
+      <c r="O57" t="str">
+        <v>Mary, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="58" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N58" t="str">
+        <v>AX, C, E, F</v>
+      </c>
+      <c r="O58" t="str">
+        <v>Mary, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="59" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N59" t="str">
+        <v>B, D, C, E, F</v>
+      </c>
+      <c r="O59" t="str">
+        <v>James, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="60" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N60" t="str">
+        <v>B, AX, D, C, E</v>
+      </c>
+      <c r="O60" t="str">
+        <v>James, Mary, Robert,X, Patricia, John</v>
+      </c>
+    </row>
+    <row r="61" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N61" t="str">
+        <v>B, AX, D, C, F</v>
+      </c>
+      <c r="O61" t="str">
+        <v>James, Mary, Robert,X, Patricia, Jennifer</v>
+      </c>
+    </row>
+    <row r="62" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N62" t="str">
+        <v>B, AX, D, E, F</v>
+      </c>
+      <c r="O62" t="str">
+        <v>James, Mary, Robert,X, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="63" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N63" t="str">
+        <v>B, AX, C, E, F</v>
+      </c>
+      <c r="O63" t="str">
+        <v>James, Mary, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="64" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N64" t="str">
+        <v>AX, D, C, E, F</v>
+      </c>
+      <c r="O64" t="str">
+        <v>Mary, Robert,X, Patricia, John, Jennifer</v>
+      </c>
+    </row>
+    <row r="65" spans="14:15" x14ac:dyDescent="0.35">
+      <c r="N65" t="str">
+        <v>B, AX, D, C, E, F</v>
+      </c>
+      <c r="O65" t="str">
         <v>James, Mary, Robert,X, Patricia, John, Jennifer</v>
       </c>
     </row>

</xml_diff>